<commit_message>
Added Owner library to read property file
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -521,7 +521,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -607,7 +609,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Added Zerocell library for Excel reading
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -521,9 +521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -609,7 +607,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Setting up selenium grid using docker
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -62,15 +62,9 @@
     <t>version</t>
   </si>
   <si>
-    <t>79.0.3945.117</t>
-  </si>
-  <si>
     <t>88.0.4324.96</t>
   </si>
   <si>
-    <t>90.0.4430.85</t>
-  </si>
-  <si>
     <t>TestName</t>
   </si>
   <si>
@@ -83,7 +77,13 @@
     <t>MenuToSelect</t>
   </si>
   <si>
-    <t>edge</t>
+    <t>98.0</t>
+  </si>
+  <si>
+    <t>firefox</t>
+  </si>
+  <si>
+    <t>97.0</t>
   </si>
 </sst>
 </file>
@@ -484,13 +484,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="28.5" x14ac:dyDescent="0.65">
       <c r="A1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="28.5" x14ac:dyDescent="0.65">
@@ -539,10 +539,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.65">
       <c r="A1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>8</v>
@@ -557,7 +557,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="28.5" x14ac:dyDescent="0.65">
@@ -571,7 +571,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>6</v>
@@ -591,10 +591,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>15</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>7</v>
@@ -617,7 +617,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Selenium grid 4 set up using docker-compose.yaml
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>loginLogoutTest</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>MenuToSelect</t>
-  </si>
-  <si>
-    <t>98.0</t>
   </si>
   <si>
     <t>firefox</t>
@@ -523,11 +520,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="38.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="30.26953125" customWidth="1"/>
     <col min="2" max="3" width="18.1796875" customWidth="1"/>
@@ -591,10 +590,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>7</v>
@@ -603,29 +602,6 @@
         <v>7</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="28.5" x14ac:dyDescent="0.65">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="1" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Docker selenium grid 4 set up for edge browser
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>loginLogoutTest</t>
   </si>
@@ -77,10 +77,10 @@
     <t>MenuToSelect</t>
   </si>
   <si>
-    <t>firefox</t>
-  </si>
-  <si>
-    <t>97.0</t>
+    <t>edge</t>
+  </si>
+  <si>
+    <t>98.0</t>
   </si>
 </sst>
 </file>
@@ -520,11 +520,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="38.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
@@ -590,7 +588,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>21</v>
@@ -602,6 +600,29 @@
         <v>7</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="28.5" x14ac:dyDescent="0.65">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>